<commit_message>
revised estimate - 17th Aug
</commit_message>
<xml_diff>
--- a/Heliusapp_project_implementation_plan.xlsx
+++ b/Heliusapp_project_implementation_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HELIUS\Documents\GitHub\projectdocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675E7E4E-4309-4686-A14F-2E4151692DB0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4B394E-CF41-4FAD-A4F7-4478A804F66D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10416" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="277">
   <si>
     <t>Task</t>
   </si>
@@ -920,6 +920,9 @@
  leaves availed. Updates the system with leave date of the employee
 2. Provides the ability to enter employee specific leave data manually by HR in case of special situations
 3.  leave elibility and utilization  data of the employees for the current year will be gathered and uploaded into system one week before feature goes live</t>
+  </si>
+  <si>
+    <t>Phase I estimate (Revised)</t>
   </si>
 </sst>
 </file>
@@ -1818,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A91" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B93" sqref="B93:D95"/>
     </sheetView>
   </sheetViews>
@@ -3791,10 +3794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A160B2E2-282E-4AB4-AF25-F319217CEA66}">
-  <dimension ref="B1:P49"/>
+  <dimension ref="B1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4983,7 +4986,7 @@
         <v>43378</v>
       </c>
     </row>
-    <row r="49" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B49" s="12" t="s">
         <v>266</v>
       </c>
@@ -4994,20 +4997,529 @@
         <v>43385</v>
       </c>
     </row>
+    <row r="52" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="N53" s="19"/>
+      <c r="O53" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P53" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="13">
+        <v>43292</v>
+      </c>
+      <c r="D54" s="13">
+        <v>43306</v>
+      </c>
+      <c r="E54" s="13">
+        <v>43307</v>
+      </c>
+      <c r="F54" s="13">
+        <v>43676</v>
+      </c>
+      <c r="G54" s="13">
+        <v>43312</v>
+      </c>
+      <c r="H54" s="13">
+        <v>43313</v>
+      </c>
+      <c r="I54" s="13">
+        <v>43314</v>
+      </c>
+      <c r="J54" s="13">
+        <v>43315</v>
+      </c>
+      <c r="K54" s="13">
+        <v>43318</v>
+      </c>
+      <c r="L54" s="13">
+        <v>43319</v>
+      </c>
+      <c r="M54" s="13">
+        <v>43320</v>
+      </c>
+      <c r="N54" s="13">
+        <v>43382</v>
+      </c>
+      <c r="O54" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P54" s="18">
+        <v>43322</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" s="13">
+        <v>43307</v>
+      </c>
+      <c r="D55" s="13">
+        <v>43315</v>
+      </c>
+      <c r="E55" s="13">
+        <v>43318</v>
+      </c>
+      <c r="F55" s="13">
+        <v>43319</v>
+      </c>
+      <c r="G55" s="13">
+        <v>43320</v>
+      </c>
+      <c r="H55" s="13">
+        <v>43321</v>
+      </c>
+      <c r="I55" s="13">
+        <v>43322</v>
+      </c>
+      <c r="J55" s="13">
+        <v>43325</v>
+      </c>
+      <c r="K55" s="13">
+        <v>43326</v>
+      </c>
+      <c r="L55" s="13">
+        <v>43326</v>
+      </c>
+      <c r="M55" s="13">
+        <v>43328</v>
+      </c>
+      <c r="N55" s="13">
+        <v>43329</v>
+      </c>
+      <c r="O55" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P55" s="18">
+        <v>43329</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="13">
+        <v>43318</v>
+      </c>
+      <c r="D56" s="13">
+        <v>43322</v>
+      </c>
+      <c r="E56" s="13">
+        <v>43332</v>
+      </c>
+      <c r="F56" s="13">
+        <v>43333</v>
+      </c>
+      <c r="G56" s="13">
+        <v>43334</v>
+      </c>
+      <c r="H56" s="13">
+        <v>43335</v>
+      </c>
+      <c r="I56" s="13">
+        <v>43336</v>
+      </c>
+      <c r="J56" s="13">
+        <v>43339</v>
+      </c>
+      <c r="K56" s="13">
+        <v>43340</v>
+      </c>
+      <c r="L56" s="13">
+        <v>43341</v>
+      </c>
+      <c r="M56" s="13">
+        <v>43342</v>
+      </c>
+      <c r="N56" s="13">
+        <v>43343</v>
+      </c>
+      <c r="O56" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P56" s="18">
+        <v>43343</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C57" s="13">
+        <v>43292</v>
+      </c>
+      <c r="D57" s="13">
+        <v>43308</v>
+      </c>
+      <c r="E57" s="13">
+        <v>43312</v>
+      </c>
+      <c r="F57" s="13">
+        <v>43314</v>
+      </c>
+      <c r="G57" s="13">
+        <v>43315</v>
+      </c>
+      <c r="H57" s="13">
+        <v>43318</v>
+      </c>
+      <c r="I57" s="13">
+        <v>43319</v>
+      </c>
+      <c r="J57" s="13">
+        <v>43321</v>
+      </c>
+      <c r="K57" s="13">
+        <v>43322</v>
+      </c>
+      <c r="L57" s="13">
+        <v>43325</v>
+      </c>
+      <c r="M57" s="13">
+        <v>43326</v>
+      </c>
+      <c r="N57" s="13">
+        <v>43329</v>
+      </c>
+      <c r="O57" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P57" s="18">
+        <v>43336</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="13">
+        <v>43325</v>
+      </c>
+      <c r="D58" s="13">
+        <v>43332</v>
+      </c>
+      <c r="E58" s="13">
+        <v>43333</v>
+      </c>
+      <c r="F58" s="13">
+        <v>43334</v>
+      </c>
+      <c r="G58" s="13">
+        <v>43335</v>
+      </c>
+      <c r="H58" s="13">
+        <v>43336</v>
+      </c>
+      <c r="I58" s="13">
+        <v>43339</v>
+      </c>
+      <c r="J58" s="13">
+        <v>43340</v>
+      </c>
+      <c r="K58" s="13">
+        <v>43341</v>
+      </c>
+      <c r="L58" s="13">
+        <v>43342</v>
+      </c>
+      <c r="M58" s="13">
+        <v>43346</v>
+      </c>
+      <c r="N58" s="13">
+        <v>43347</v>
+      </c>
+      <c r="O58" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P58" s="18">
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" s="13">
+        <v>43333</v>
+      </c>
+      <c r="D59" s="13">
+        <v>43341</v>
+      </c>
+      <c r="E59" s="13">
+        <v>43342</v>
+      </c>
+      <c r="F59" s="13">
+        <v>43343</v>
+      </c>
+      <c r="G59" s="13">
+        <v>43344</v>
+      </c>
+      <c r="H59" s="13">
+        <v>43345</v>
+      </c>
+      <c r="I59" s="13">
+        <v>43346</v>
+      </c>
+      <c r="J59" s="13">
+        <v>43347</v>
+      </c>
+      <c r="K59" s="13">
+        <v>43348</v>
+      </c>
+      <c r="L59" s="13">
+        <v>43351</v>
+      </c>
+      <c r="M59" s="13">
+        <v>43352</v>
+      </c>
+      <c r="N59" s="13">
+        <v>43353</v>
+      </c>
+      <c r="O59" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P59" s="18">
+        <v>43357</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="13">
+        <v>43342</v>
+      </c>
+      <c r="D60" s="13">
+        <v>43357</v>
+      </c>
+      <c r="E60" s="13">
+        <v>43360</v>
+      </c>
+      <c r="F60" s="13">
+        <v>43361</v>
+      </c>
+      <c r="G60" s="13">
+        <v>43362</v>
+      </c>
+      <c r="H60" s="13">
+        <v>43363</v>
+      </c>
+      <c r="I60" s="13">
+        <v>43367</v>
+      </c>
+      <c r="J60" s="13">
+        <v>43368</v>
+      </c>
+      <c r="K60" s="13">
+        <v>43369</v>
+      </c>
+      <c r="L60" s="13">
+        <v>43370</v>
+      </c>
+      <c r="M60" s="13">
+        <v>43371</v>
+      </c>
+      <c r="N60" s="13">
+        <v>43374</v>
+      </c>
+      <c r="O60" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P60" s="18">
+        <v>43374</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="13">
+        <v>43342</v>
+      </c>
+      <c r="D61" s="13">
+        <v>43357</v>
+      </c>
+      <c r="E61" s="13">
+        <v>43360</v>
+      </c>
+      <c r="F61" s="13">
+        <v>43361</v>
+      </c>
+      <c r="G61" s="13">
+        <v>43362</v>
+      </c>
+      <c r="H61" s="13">
+        <v>43363</v>
+      </c>
+      <c r="I61" s="13">
+        <v>43367</v>
+      </c>
+      <c r="J61" s="13">
+        <v>43368</v>
+      </c>
+      <c r="K61" s="13">
+        <v>43369</v>
+      </c>
+      <c r="L61" s="13">
+        <v>43370</v>
+      </c>
+      <c r="M61" s="13">
+        <v>43371</v>
+      </c>
+      <c r="N61" s="13">
+        <v>43374</v>
+      </c>
+      <c r="O61" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P61" s="18">
+        <v>43378</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C62" s="18">
+        <v>43360</v>
+      </c>
+      <c r="D62" s="18">
+        <v>43369</v>
+      </c>
+      <c r="E62" s="18">
+        <v>43370</v>
+      </c>
+      <c r="F62" s="18">
+        <v>43371</v>
+      </c>
+      <c r="G62" s="18">
+        <v>43374</v>
+      </c>
+      <c r="H62" s="18">
+        <v>43376</v>
+      </c>
+      <c r="I62" s="18">
+        <v>43377</v>
+      </c>
+      <c r="J62" s="18">
+        <v>43378</v>
+      </c>
+      <c r="K62" s="18">
+        <v>43381</v>
+      </c>
+      <c r="L62" s="18">
+        <v>43382</v>
+      </c>
+      <c r="M62" s="18">
+        <v>43383</v>
+      </c>
+      <c r="N62" s="18">
+        <v>43384</v>
+      </c>
+      <c r="O62" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="P62" s="18">
+        <v>43385</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="12"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="13"/>
+      <c r="L63" s="13"/>
+      <c r="M63" s="13"/>
+      <c r="N63" s="13"/>
+      <c r="P63" s="8"/>
+    </row>
+    <row r="64" spans="2:16" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="13"/>
+    </row>
+    <row r="65" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C65" s="13"/>
+    </row>
+    <row r="66" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="13"/>
+    </row>
+    <row r="67" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="13"/>
+    </row>
+    <row r="68" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C68" s="13"/>
+    </row>
+    <row r="69" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="D69" s="10">
+        <v>43378</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M53:N53"/>
     <mergeCell ref="M21:N21"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="K21:L21"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="K53:L53"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" location="timesheets!A1" display="RTS timesheet" xr:uid="{64988F1E-7502-449B-BE66-02320B324CDA}"/>
@@ -5028,16 +5540,24 @@
     <hyperlink ref="B22" location="Employeemaster!A1" display="Employee master" xr:uid="{81D930A9-D162-44FD-9AFD-0C36E349123A}"/>
     <hyperlink ref="B24" location="'Phase1-HR-Employeejourney'!A1" display="ExitEmployee" xr:uid="{EFD3782A-BED1-4B83-8E00-6E521B8539B9}"/>
     <hyperlink ref="B23" location="'Phase1-HR-Employeejourney'!A1" display="onboarding documents" xr:uid="{033DDE7F-6783-4B6B-BBAC-0C0A1B22AD4F}"/>
-    <hyperlink ref="B41" location="Employeemaster!A1" display="Employee master" xr:uid="{6468CA02-5134-4009-A6F7-DEAA3259654E}"/>
-    <hyperlink ref="B42" location="'Phase1-HR-Employeejourney'!A1" display="onboarding documents" xr:uid="{082F7B7F-A1ED-4553-AAD9-D1038B4A8CF0}"/>
-    <hyperlink ref="B43" location="'Phase1-HR-Employeejourney'!A1" display="ExitEmployee" xr:uid="{BA4F232D-2023-4869-9E8C-1334B3C71041}"/>
-    <hyperlink ref="B44" location="'Phase1-HR-Employeejourney'!A1" display="Clientmaster" xr:uid="{52A6DACA-C7F7-42D0-8DA4-00CD34459261}"/>
     <hyperlink ref="B30" location="'Phase1-HR-Employeejourney'!A1" display="ApplyMeritincrease" xr:uid="{0DC47E64-8204-4583-A871-42D621BE0AFB}"/>
-    <hyperlink ref="B45" location="'Phase1-HR-Employeejourney'!A1" display="RTS timesheet" xr:uid="{1DDC1CB4-2728-436A-8746-56FC460BD197}"/>
     <hyperlink ref="B46" location="timesheets!A1" display="Manual timesheet" xr:uid="{3EAA65B1-0DCD-4058-B1C4-764E9D82E606}"/>
     <hyperlink ref="B47" location="Leaves!A1" display="Leaves" xr:uid="{84BD21A3-CE76-49CE-82D1-3B9B3BEFC487}"/>
     <hyperlink ref="B48" location="Claims!A1" display="Claims" xr:uid="{8076CE51-ECF5-41B6-AFD8-3D638DCED36D}"/>
     <hyperlink ref="B49" location="'Phase1-HR-Employeejourney'!A1" display="ApplyMeritincrease" xr:uid="{7C69E4F8-4559-4FBF-A879-DD7E87B94A01}"/>
+    <hyperlink ref="B45" location="'Phase1-HR-Employeejourney'!A1" display="RTS timesheet" xr:uid="{1DDC1CB4-2728-436A-8746-56FC460BD197}"/>
+    <hyperlink ref="B44" location="'Phase1-HR-Employeejourney'!A1" display="Clientmaster" xr:uid="{52A6DACA-C7F7-42D0-8DA4-00CD34459261}"/>
+    <hyperlink ref="B43" location="'Phase1-HR-Employeejourney'!A1" display="ExitEmployee" xr:uid="{BA4F232D-2023-4869-9E8C-1334B3C71041}"/>
+    <hyperlink ref="B42" location="'Phase1-HR-Employeejourney'!A1" display="onboarding documents" xr:uid="{082F7B7F-A1ED-4553-AAD9-D1038B4A8CF0}"/>
+    <hyperlink ref="B41" location="Employeemaster!A1" display="Employee master" xr:uid="{6468CA02-5134-4009-A6F7-DEAA3259654E}"/>
+    <hyperlink ref="B58" location="timesheets!A1" display="RTS timesheet" xr:uid="{C90FD3BC-E33C-43B8-9EBC-F0174EC16B92}"/>
+    <hyperlink ref="B59" location="timesheets!A1" display="Manual timesheet" xr:uid="{1907642F-7962-47DB-8AE9-5314AE9407BB}"/>
+    <hyperlink ref="B60" location="Leaves!A1" display="Leaves" xr:uid="{5C116E2F-F90F-443F-8ABF-CD4DB2CD3CBB}"/>
+    <hyperlink ref="B61" location="Claims!A1" display="Claims" xr:uid="{DD7E3323-134C-42A1-982F-BD363E6A21B6}"/>
+    <hyperlink ref="B54" location="Employeemaster!A1" display="Employee master" xr:uid="{3F556829-AADF-460B-BB27-AFB552F3099F}"/>
+    <hyperlink ref="B56" location="'Phase1-HR-Employeejourney'!A1" display="ExitEmployee" xr:uid="{12D33AC8-87C4-46B5-B61B-69D0729708E3}"/>
+    <hyperlink ref="B55" location="'Phase1-HR-Employeejourney'!A1" display="onboarding documents" xr:uid="{6BF20465-E5B3-4395-91EC-C726A961CF3B}"/>
+    <hyperlink ref="B62" location="'Phase1-HR-Employeejourney'!A1" display="ApplyMeritincrease" xr:uid="{EB83343A-3C90-4DAC-84F0-8C78466AA507}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>